<commit_message>
Remarks : file updated with tc no - 19,20
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_Chart.xlsx
+++ b/TCS_NEWUI_Chart.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\Completed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CA4F5D-9AA7-4532-B1C7-BF852CEB8B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -46,7 +40,7 @@
     <definedName name="test" localSheetId="1">#REF!</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="204">
   <si>
     <t>Test Case Result Modules-Wise</t>
   </si>
@@ -792,11 +786,61 @@
 2. Reset button should be Enabled
 3. Save button should not be Enabled</t>
   </si>
+  <si>
+    <t>SMRT-8033</t>
+  </si>
+  <si>
+    <t>Verify on selecting chart option from All Analytics drop down should hide granular data in Brand Monthly charts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC20 </t>
+  </si>
+  <si>
+    <t>Verify the Expand Functionality should hide granular data in Brand Monthly reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC19 </t>
+  </si>
+  <si>
+    <t>1. Chart should be expanded
+2. Chart's all other remaining bar value should be displayed
+3. Expand button turn into  "Go Back" button
+4. AgGrid should not be displayed below chart for granular data</t>
+  </si>
+  <si>
+    <t>Click on All Analytics drop down button and select Company Ranking Period over Period</t>
+  </si>
+  <si>
+    <t>Chart -Company Ranking Period over Period,Leading Class Media Mix… for all charts with Expand button</t>
+  </si>
+  <si>
+    <t>UA - Brand Monthly
+Report -QA Testing - Ad Ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should on Home screen of the application.
+Home screen should contain below section:
+1. Numerator logo on Top Left side of screen
+2. Report list on left side
+3. Total creatives chart
+4. Saved search list
+5. Chart as per current date filter
+6. Save and Reset button should be displayed as Disabled on Right side
+7. Breadcrumb below creative Chart
+8. Export Result &amp; Search options button on Right bottom side
+</t>
+  </si>
+  <si>
+    <t>US:WEB-7575_TC 20</t>
+  </si>
+  <si>
+    <t>US:WEB-7575_TC 19</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -2271,7 +2315,7 @@
     <xf numFmtId="41" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="92" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="134"/>
@@ -2508,164 +2552,168 @@
     <xf numFmtId="0" fontId="45" fillId="29" borderId="39" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="152" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="152" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="156">
-    <cellStyle name="20% - Accent1" xfId="11" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3" xfId="13" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent1 2 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 4" xfId="29" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - Accent2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3" xfId="34" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - Accent2 2 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="20% - Accent2 2 3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="20% - Accent5" xfId="42" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - Accent6" xfId="16" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="40% - Accent1" xfId="3" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="40% - Accent1 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="40% - Accent1 2 3" xfId="54" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="40% - Accent1 2 3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="40% - Accent2" xfId="12" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="40% - Accent2 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2 3" xfId="31" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="40% - Accent2 2 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2 2" xfId="138" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="40% - Accent3" xfId="6" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="40% - Accent4" xfId="21" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="40% - Accent5" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="40% - Accent6" xfId="53" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="60% - Accent1" xfId="41" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="60% - Accent2" xfId="14" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="60% - Accent3" xfId="18" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="60% - Accent4" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="60% - Accent5" xfId="63" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="60% - Accent6" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Accent1" xfId="64" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Accent1 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Accent1 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Accent1 2 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Accent1 2 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Accent1 2 3 2 2" xfId="135" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Accent2" xfId="70" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Accent2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Accent2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3 3" xfId="73" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Accent2 2 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Accent2 2 3 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent2 2 3 2 2" xfId="136" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Accent3" xfId="76" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Accent4" xfId="23" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Accent5" xfId="77" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Accent6" xfId="26" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Bad" xfId="78" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Calculation" xfId="8" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Check Cell" xfId="79" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Comma [0] 2" xfId="154" xr:uid="{0A0E39A6-308B-42DF-BD5C-F7C342AF9AF2}"/>
-    <cellStyle name="Comma [0] 3" xfId="155" xr:uid="{FE889529-AB91-400A-92C4-677C94A70BEE}"/>
-    <cellStyle name="Explanatory Text" xfId="80" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Good" xfId="81" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Heading 1" xfId="82" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Heading 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Heading 2 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Heading 2 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2 3" xfId="89" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Heading 2 2 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Heading 2 2 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Heading 3" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Heading 4" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="20% - Accent1" xfId="11"/>
+    <cellStyle name="20% - Accent1 2" xfId="2"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="7"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3" xfId="13"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3 2" xfId="17"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3 3" xfId="20"/>
+    <cellStyle name="20% - Accent1 2 3" xfId="22"/>
+    <cellStyle name="20% - Accent1 2 3 2" xfId="25"/>
+    <cellStyle name="20% - Accent1 2 3 2 2" xfId="28"/>
+    <cellStyle name="20% - Accent1 2 3 2 3" xfId="5"/>
+    <cellStyle name="20% - Accent1 2 3 2 4" xfId="29"/>
+    <cellStyle name="20% - Accent2" xfId="30"/>
+    <cellStyle name="20% - Accent2 2" xfId="32"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="33"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3" xfId="34"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3 2" xfId="36"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3 3" xfId="37"/>
+    <cellStyle name="20% - Accent2 2 3" xfId="35"/>
+    <cellStyle name="20% - Accent2 2 3 2" xfId="9"/>
+    <cellStyle name="20% - Accent3" xfId="39"/>
+    <cellStyle name="20% - Accent4" xfId="40"/>
+    <cellStyle name="20% - Accent5" xfId="42"/>
+    <cellStyle name="20% - Accent6" xfId="16"/>
+    <cellStyle name="40% - Accent1" xfId="3"/>
+    <cellStyle name="40% - Accent1 2" xfId="43"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="45"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2" xfId="48"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2 2" xfId="51"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2 3" xfId="52"/>
+    <cellStyle name="40% - Accent1 2 3" xfId="54"/>
+    <cellStyle name="40% - Accent1 2 3 2" xfId="55"/>
+    <cellStyle name="40% - Accent2" xfId="12"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="38"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2" xfId="60"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2 2" xfId="62"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2 3" xfId="31"/>
+    <cellStyle name="40% - Accent2 2 3" xfId="58"/>
+    <cellStyle name="40% - Accent2 2 3 2" xfId="61"/>
+    <cellStyle name="40% - Accent2 2 3 2 2" xfId="138"/>
+    <cellStyle name="40% - Accent2 2 3 2 2 2" xfId="150"/>
+    <cellStyle name="40% - Accent3" xfId="6"/>
+    <cellStyle name="40% - Accent4" xfId="21"/>
+    <cellStyle name="40% - Accent5" xfId="44"/>
+    <cellStyle name="40% - Accent6" xfId="53"/>
+    <cellStyle name="60% - Accent1" xfId="41"/>
+    <cellStyle name="60% - Accent2" xfId="14"/>
+    <cellStyle name="60% - Accent3" xfId="18"/>
+    <cellStyle name="60% - Accent4" xfId="47"/>
+    <cellStyle name="60% - Accent5" xfId="63"/>
+    <cellStyle name="60% - Accent6" xfId="50"/>
+    <cellStyle name="Accent1" xfId="64"/>
+    <cellStyle name="Accent1 2" xfId="65"/>
+    <cellStyle name="Accent1 2 2" xfId="57"/>
+    <cellStyle name="Accent1 2 2 2 2 3" xfId="24"/>
+    <cellStyle name="Accent1 2 2 2 2 3 2" xfId="27"/>
+    <cellStyle name="Accent1 2 2 2 2 3 3" xfId="4"/>
+    <cellStyle name="Accent1 2 3" xfId="66"/>
+    <cellStyle name="Accent1 2 3 2" xfId="69"/>
+    <cellStyle name="Accent1 2 3 2 2" xfId="135"/>
+    <cellStyle name="Accent2" xfId="70"/>
+    <cellStyle name="Accent2 2" xfId="46"/>
+    <cellStyle name="Accent2 2 2" xfId="49"/>
+    <cellStyle name="Accent2 2 2 2 2 3" xfId="71"/>
+    <cellStyle name="Accent2 2 2 2 2 3 2" xfId="72"/>
+    <cellStyle name="Accent2 2 2 2 2 3 3" xfId="73"/>
+    <cellStyle name="Accent2 2 3" xfId="74"/>
+    <cellStyle name="Accent2 2 3 2" xfId="75"/>
+    <cellStyle name="Accent2 2 3 2 2" xfId="136"/>
+    <cellStyle name="Accent3" xfId="76"/>
+    <cellStyle name="Accent4" xfId="23"/>
+    <cellStyle name="Accent5" xfId="77"/>
+    <cellStyle name="Accent6" xfId="26"/>
+    <cellStyle name="Bad" xfId="78"/>
+    <cellStyle name="Calculation" xfId="8"/>
+    <cellStyle name="Check Cell" xfId="79"/>
+    <cellStyle name="Comma [0] 2" xfId="154"/>
+    <cellStyle name="Comma [0] 3" xfId="155"/>
+    <cellStyle name="Explanatory Text" xfId="80"/>
+    <cellStyle name="Good" xfId="81"/>
+    <cellStyle name="Heading 1" xfId="82"/>
+    <cellStyle name="Heading 2" xfId="84"/>
+    <cellStyle name="Heading 2 2" xfId="85"/>
+    <cellStyle name="Heading 2 2 2" xfId="86"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="87"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2 2" xfId="88"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2 3" xfId="89"/>
+    <cellStyle name="Heading 2 2 3" xfId="10"/>
+    <cellStyle name="Heading 2 2 3 2" xfId="1"/>
+    <cellStyle name="Heading 3" xfId="90"/>
+    <cellStyle name="Heading 4" xfId="91"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="95" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Hyperlink 4" xfId="96" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Hyperlink 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Input" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Linked Cell" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Neutral" xfId="59" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="93"/>
+    <cellStyle name="Hyperlink 2 2" xfId="94"/>
+    <cellStyle name="Hyperlink 3" xfId="95"/>
+    <cellStyle name="Hyperlink 4" xfId="96"/>
+    <cellStyle name="Hyperlink 5" xfId="137"/>
+    <cellStyle name="Input" xfId="97"/>
+    <cellStyle name="Linked Cell" xfId="98"/>
+    <cellStyle name="Neutral" xfId="59"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2 3" xfId="104" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 2 3" xfId="105" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 2 4" xfId="106" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 2 4 2" xfId="134" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 2 4 2 2" xfId="149" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 3" xfId="107" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 3 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="109" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 3 2 4" xfId="140" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 3 2 4 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 3 2 4 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 3 2 4 3 2" xfId="152" xr:uid="{32E79525-A200-4DBB-8CA8-2DD8C8431D53}"/>
-    <cellStyle name="Normal 3 3" xfId="56" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 3 4" xfId="139" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="151" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 4" xfId="113" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 5" xfId="114" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Note" xfId="68" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Output" xfId="19" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="TableStyleLight1" xfId="115" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="TableStyleLight1 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="TableStyleLight1 2 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2 4" xfId="120" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="TableStyleLight1 2 3" xfId="121" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="TableStyleLight1 2 4" xfId="142" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="TableStyleLight1 2 4 2" xfId="145" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="TableStyleLight1 2 4 3" xfId="148" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="TableStyleLight1 3" xfId="122" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="TableStyleLight1 3 2" xfId="123" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="TableStyleLight1 3 2 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="TableStyleLight1 3 2 3" xfId="125" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="TableStyleLight1 3 3" xfId="126" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="TableStyleLight1 3 4" xfId="141" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 2" xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="153" xr:uid="{11E5449E-3D73-4B06-8B4C-9895ECFB313A}"/>
-    <cellStyle name="TableStyleLight1 4" xfId="67" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="TableStyleLight1 4 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="TableStyleLight1 4 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="TableStyleLight1 5" xfId="129" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="TableStyleLight1 5 2" xfId="130" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Title" xfId="131" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Total" xfId="132" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Warning Text" xfId="133" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 2" xfId="99"/>
+    <cellStyle name="Normal 2 2" xfId="100"/>
+    <cellStyle name="Normal 2 2 2" xfId="101"/>
+    <cellStyle name="Normal 2 2 2 2 3 2" xfId="102"/>
+    <cellStyle name="Normal 2 2 2 2 3 2 2" xfId="103"/>
+    <cellStyle name="Normal 2 2 2 2 3 2 3" xfId="104"/>
+    <cellStyle name="Normal 2 3" xfId="105"/>
+    <cellStyle name="Normal 2 4" xfId="106"/>
+    <cellStyle name="Normal 2 4 2" xfId="134"/>
+    <cellStyle name="Normal 2 4 2 2" xfId="149"/>
+    <cellStyle name="Normal 3" xfId="107"/>
+    <cellStyle name="Normal 3 2" xfId="108"/>
+    <cellStyle name="Normal 3 2 2" xfId="109"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="110"/>
+    <cellStyle name="Normal 3 2 4" xfId="140"/>
+    <cellStyle name="Normal 3 2 4 2" xfId="143"/>
+    <cellStyle name="Normal 3 2 4 3" xfId="146"/>
+    <cellStyle name="Normal 3 2 4 3 2" xfId="152"/>
+    <cellStyle name="Normal 3 3" xfId="56"/>
+    <cellStyle name="Normal 3 3 2" xfId="111"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="112"/>
+    <cellStyle name="Normal 3 4" xfId="139"/>
+    <cellStyle name="Normal 3 4 2" xfId="151"/>
+    <cellStyle name="Normal 4" xfId="113"/>
+    <cellStyle name="Normal 5" xfId="114"/>
+    <cellStyle name="Note" xfId="68"/>
+    <cellStyle name="Output" xfId="19"/>
+    <cellStyle name="TableStyleLight1" xfId="115"/>
+    <cellStyle name="TableStyleLight1 2" xfId="116"/>
+    <cellStyle name="TableStyleLight1 2 2" xfId="117"/>
+    <cellStyle name="TableStyleLight1 2 2 2" xfId="118"/>
+    <cellStyle name="TableStyleLight1 2 2 2 2" xfId="119"/>
+    <cellStyle name="TableStyleLight1 2 2 2 4" xfId="120"/>
+    <cellStyle name="TableStyleLight1 2 3" xfId="121"/>
+    <cellStyle name="TableStyleLight1 2 4" xfId="142"/>
+    <cellStyle name="TableStyleLight1 2 4 2" xfId="145"/>
+    <cellStyle name="TableStyleLight1 2 4 3" xfId="148"/>
+    <cellStyle name="TableStyleLight1 3" xfId="122"/>
+    <cellStyle name="TableStyleLight1 3 2" xfId="123"/>
+    <cellStyle name="TableStyleLight1 3 2 2" xfId="124"/>
+    <cellStyle name="TableStyleLight1 3 2 3" xfId="125"/>
+    <cellStyle name="TableStyleLight1 3 3" xfId="126"/>
+    <cellStyle name="TableStyleLight1 3 4" xfId="141"/>
+    <cellStyle name="TableStyleLight1 3 4 2" xfId="144"/>
+    <cellStyle name="TableStyleLight1 3 4 3" xfId="147"/>
+    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="153"/>
+    <cellStyle name="TableStyleLight1 4" xfId="67"/>
+    <cellStyle name="TableStyleLight1 4 2" xfId="127"/>
+    <cellStyle name="TableStyleLight1 4 3" xfId="128"/>
+    <cellStyle name="TableStyleLight1 5" xfId="129"/>
+    <cellStyle name="TableStyleLight1 5 2" xfId="130"/>
+    <cellStyle name="Title" xfId="131"/>
+    <cellStyle name="Total" xfId="132"/>
+    <cellStyle name="Warning Text" xfId="133"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2752,18 +2800,10 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="148"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="48"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="48"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2786,25 +2826,22 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.3923741222529194E-2"/>
-          <c:y val="0.1418565099457787"/>
+          <c:x val="5.3923741222529187E-2"/>
+          <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321821"/>
+          <c:h val="0.75521895211321832"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2819,11 +2856,8 @@
               <a:bevelT w="63500" h="25400"/>
             </a:sp3d>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2840,7 +2874,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2848,8 +2882,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="E22B00"/>
@@ -2864,7 +2896,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2872,8 +2904,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -2888,7 +2918,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2896,8 +2926,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -2912,7 +2940,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2936,14 +2964,8 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2976,7 +2998,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -2990,34 +3012,23 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1420334192"/>
-        <c:axId val="1420343440"/>
+        <c:dLbls/>
+        <c:axId val="49907584"/>
+        <c:axId val="49909120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1420334192"/>
+        <c:axId val="49907584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3031,32 +3042,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1420343440"/>
+        <c:crossAx val="49909120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1420343440"/>
+        <c:axId val="49909120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1420334192"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="49907584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:effectLst/>
@@ -3070,25 +3077,17 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="145"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="45"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="45"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3111,24 +3110,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="32"/>
-      <c:rAngAx val="0"/>
       <c:perspective val="90"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3136,9 +3123,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603381"/>
-          <c:w val="0.92496729254319687"/>
-          <c:h val="0.69766331701963358"/>
+          <c:y val="0.14624350369603384"/>
+          <c:w val="0.92496729254319709"/>
+          <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -3148,7 +3135,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -3157,7 +3143,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-700B-4388-A157-532FE5806D3B}"/>
               </c:ext>
@@ -3165,7 +3151,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:explosion val="19"/>
             <c:spPr>
               <a:solidFill>
@@ -3175,7 +3160,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-700B-4388-A157-532FE5806D3B}"/>
               </c:ext>
@@ -3199,17 +3184,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-700B-4388-A157-532FE5806D3B}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -3228,17 +3202,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-700B-4388-A157-532FE5806D3B}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
@@ -3247,14 +3210,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3279,28 +3237,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16666666666666663</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-700B-4388-A157-532FE5806D3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
       </c:pie3DChart>
       <c:spPr>
@@ -3316,16 +3268,14 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253508"/>
-          <c:w val="0.42791036796598075"/>
+          <c:y val="0.88141746683253497"/>
+          <c:w val="0.42791036796598092"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln w="0"/>
@@ -3339,7 +3289,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -3347,20 +3297,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3368,9 +3307,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686355E-2"/>
-          <c:w val="0.29672375522792593"/>
-          <c:h val="0.85466509216403797"/>
+          <c:y val="7.1365887012686369E-2"/>
+          <c:w val="0.29672375522792599"/>
+          <c:h val="0.85466509216403819"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -3385,7 +3324,6 @@
           </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="92D050"/>
@@ -3394,7 +3332,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-25D4-4E58-AB57-52CC97BAF3DE}"/>
               </c:ext>
@@ -3402,7 +3340,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -3411,7 +3348,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-25D4-4E58-AB57-52CC97BAF3DE}"/>
               </c:ext>
@@ -3419,7 +3356,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -3428,7 +3364,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-25D4-4E58-AB57-52CC97BAF3DE}"/>
               </c:ext>
@@ -3436,7 +3372,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -3445,7 +3380,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-25D4-4E58-AB57-52CC97BAF3DE}"/>
               </c:ext>
@@ -3478,7 +3413,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -3492,21 +3427,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-25D4-4E58-AB57-52CC97BAF3DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -3587,13 +3514,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72165251246917395"/>
-          <c:y val="3.608395161789857E-3"/>
+          <c:x val="0.72165251246917417"/>
+          <c:y val="3.6083951617898579E-3"/>
           <c:w val="0.24112408909611374"/>
-          <c:h val="0.95693837006674265"/>
+          <c:h val="0.95693837006674254"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -3620,7 +3546,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3652,7 +3577,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3678,7 +3603,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3716,7 +3641,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3754,7 +3679,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3763,10 +3688,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3786,7 +3711,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3858,7 +3783,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3992,7 +3917,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4042,7 +3967,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4393,7 +4318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4461,7 +4386,7 @@
       </c>
       <c r="B8" s="12">
         <f>'SMART- Chart'!G7</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="12">
         <f>'SMART- Chart'!G8</f>
@@ -4477,11 +4402,11 @@
       </c>
       <c r="F8" s="12">
         <f>SUM(B8:E8)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G8" s="17">
         <f>(B8+C8+D8)/(F8)</f>
-        <v>0.83333333333333337</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4499,7 +4424,7 @@
       </c>
       <c r="B10" s="18">
         <f>SUM(B8:B9)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" s="18">
         <f>SUM(C8:C9)</f>
@@ -4515,11 +4440,11 @@
       </c>
       <c r="F10" s="18">
         <f>SUM(F8:F9)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G10" s="14">
         <f>SUM(G8:G8)</f>
-        <v>0.83333333333333337</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickTop="1">
@@ -4528,7 +4453,7 @@
       </c>
       <c r="G11" s="15">
         <f>100%-G10</f>
-        <v>0.16666666666666663</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4542,7 +4467,7 @@
     <mergeCell ref="G6:G7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A8" location="'SMART- Chart'!A1" display="SMART-Chart" xr:uid="{3C04F7C3-0903-46F9-957B-F0A8B92B010E}"/>
+    <hyperlink ref="A8" location="'SMART- Chart'!A1" display="SMART-Chart"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4551,11 +4476,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5028,16 +4953,28 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="77"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
+      <c r="B20" s="94" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="93" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
+        <v>192</v>
+      </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="77"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
+      <c r="B21" s="94" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="93" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
+        <v>192</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
@@ -5340,10 +5277,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14479089-7CD9-4D53-9264-25F770CD02CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H969"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -6089,8 +6028,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="32">
-        <f>COUNTIF(G11:G1095,"Pass")</f>
-        <v>11</v>
+        <f>COUNTIF(G11:G2000,"Pass")</f>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
@@ -6105,7 +6044,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="32">
-        <f>COUNTIF(G12:G1096,"Fail")</f>
+        <f>COUNTIF(G12:G2000,"Fail")</f>
         <v>4</v>
       </c>
     </row>
@@ -6150,7 +6089,7 @@
       </c>
       <c r="C11" s="23">
         <f>G7</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="21"/>
@@ -8649,130 +8588,244 @@
       <c r="G158" s="80"/>
     </row>
     <row r="159" spans="1:7">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
-      <c r="D159"/>
-      <c r="E159"/>
-      <c r="F159"/>
-      <c r="G159"/>
+      <c r="A159" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="B159" s="81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C159" s="82"/>
+      <c r="D159" s="82"/>
+      <c r="E159" s="83"/>
+      <c r="F159" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="G159" s="47" t="str">
+        <f>IF(COUNTIF(F162:F164,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F162:F164,"Fail")&gt;0,"Fail",IF(COUNTIF(F162:F164,"")=0,"Pass","Not Executed")))</f>
+        <v>Pass</v>
+      </c>
     </row>
     <row r="160" spans="1:7">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="D160"/>
-      <c r="E160"/>
-      <c r="F160"/>
-      <c r="G160"/>
+      <c r="A160" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B160" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C160" s="85"/>
+      <c r="D160" s="85"/>
+      <c r="E160" s="85"/>
+      <c r="F160" s="85"/>
+      <c r="G160" s="86"/>
     </row>
     <row r="161" spans="1:7">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="D161"/>
-      <c r="E161"/>
-      <c r="F161"/>
-      <c r="G161"/>
-    </row>
-    <row r="162" spans="1:7">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="C162"/>
-      <c r="D162"/>
-      <c r="E162"/>
-      <c r="F162"/>
-      <c r="G162"/>
-    </row>
-    <row r="163" spans="1:7">
-      <c r="A163"/>
-      <c r="B163"/>
-      <c r="C163"/>
-      <c r="D163"/>
-      <c r="E163"/>
-      <c r="F163"/>
-      <c r="G163"/>
-    </row>
-    <row r="164" spans="1:7">
-      <c r="A164"/>
-      <c r="B164"/>
-      <c r="C164"/>
-      <c r="D164"/>
-      <c r="E164"/>
-      <c r="F164"/>
-      <c r="G164"/>
+      <c r="A161" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B161" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C161" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D161" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E161" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="F161" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G161" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="150">
+      <c r="A162" s="50">
+        <v>1</v>
+      </c>
+      <c r="B162" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C162" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D162" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="E162" s="52"/>
+      <c r="F162" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G162" s="54"/>
+    </row>
+    <row r="163" spans="1:7" ht="105">
+      <c r="A163" s="50">
+        <v>2</v>
+      </c>
+      <c r="B163" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C163" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D163" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="E163" s="52"/>
+      <c r="F163" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G163" s="54"/>
+    </row>
+    <row r="164" spans="1:7" ht="60">
+      <c r="A164" s="50">
+        <v>3</v>
+      </c>
+      <c r="B164" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C164" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D164" s="52"/>
+      <c r="E164" s="52"/>
+      <c r="F164" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G164" s="54"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165"/>
-      <c r="B165"/>
-      <c r="C165"/>
-      <c r="D165"/>
-      <c r="E165"/>
-      <c r="F165"/>
-      <c r="G165"/>
+      <c r="A165" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B165" s="78"/>
+      <c r="C165" s="79"/>
+      <c r="D165" s="79"/>
+      <c r="E165" s="79"/>
+      <c r="F165" s="79"/>
+      <c r="G165" s="80"/>
     </row>
     <row r="166" spans="1:7">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="C166"/>
-      <c r="D166"/>
-      <c r="E166"/>
-      <c r="F166"/>
-      <c r="G166"/>
+      <c r="A166" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B166" s="81" t="s">
+        <v>193</v>
+      </c>
+      <c r="C166" s="82"/>
+      <c r="D166" s="82"/>
+      <c r="E166" s="83"/>
+      <c r="F166" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="G166" s="47" t="str">
+        <f>IF(COUNTIF(F169:F171,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F169:F171,"Fail")&gt;0,"Fail",IF(COUNTIF(F169:F171,"")=0,"Pass","Not Executed")))</f>
+        <v>Pass</v>
+      </c>
     </row>
     <row r="167" spans="1:7">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="C167"/>
-      <c r="D167"/>
-      <c r="E167"/>
-      <c r="F167"/>
-      <c r="G167"/>
+      <c r="A167" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B167" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C167" s="85"/>
+      <c r="D167" s="85"/>
+      <c r="E167" s="85"/>
+      <c r="F167" s="85"/>
+      <c r="G167" s="86"/>
     </row>
     <row r="168" spans="1:7">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="C168"/>
-      <c r="D168"/>
-      <c r="E168"/>
-      <c r="F168"/>
-      <c r="G168"/>
+      <c r="A168" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B168" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C168" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D168" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E168" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="F168" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G168" s="49" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="169" spans="1:7" ht="30.95" customHeight="1">
-      <c r="A169"/>
-      <c r="B169"/>
-      <c r="C169"/>
-      <c r="D169"/>
-      <c r="E169"/>
-      <c r="F169"/>
-      <c r="G169"/>
-    </row>
-    <row r="170" spans="1:7">
-      <c r="A170"/>
-      <c r="B170"/>
-      <c r="C170"/>
-      <c r="D170"/>
-      <c r="E170"/>
-      <c r="F170"/>
-      <c r="G170"/>
-    </row>
-    <row r="171" spans="1:7">
-      <c r="A171"/>
-      <c r="B171"/>
-      <c r="C171"/>
-      <c r="D171"/>
-      <c r="E171"/>
-      <c r="F171"/>
-      <c r="G171"/>
+      <c r="A169" s="50">
+        <v>1</v>
+      </c>
+      <c r="B169" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C169" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="D169" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="E169" s="52"/>
+      <c r="F169" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G169" s="54"/>
+    </row>
+    <row r="170" spans="1:7" ht="105">
+      <c r="A170" s="50">
+        <v>2</v>
+      </c>
+      <c r="B170" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C170" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D170" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="E170" s="52"/>
+      <c r="F170" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G170" s="54"/>
+    </row>
+    <row r="171" spans="1:7" ht="60">
+      <c r="A171" s="50">
+        <v>3</v>
+      </c>
+      <c r="B171" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="C171" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D171" s="52"/>
+      <c r="E171" s="52"/>
+      <c r="F171" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G171" s="54"/>
     </row>
     <row r="172" spans="1:7">
-      <c r="A172"/>
-      <c r="B172"/>
-      <c r="C172"/>
-      <c r="D172"/>
-      <c r="E172"/>
-      <c r="F172"/>
-      <c r="G172"/>
+      <c r="A172" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B172" s="78"/>
+      <c r="C172" s="79"/>
+      <c r="D172" s="79"/>
+      <c r="E172" s="79"/>
+      <c r="F172" s="79"/>
+      <c r="G172" s="80"/>
     </row>
     <row r="173" spans="1:7">
       <c r="A173"/>
@@ -15945,7 +15998,55 @@
       <c r="H969" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="64">
+    <mergeCell ref="B172:G172"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="B160:G160"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="B166:E166"/>
+    <mergeCell ref="B167:G167"/>
+    <mergeCell ref="B158:G158"/>
+    <mergeCell ref="B144:E144"/>
+    <mergeCell ref="B145:G145"/>
+    <mergeCell ref="B151:G151"/>
+    <mergeCell ref="B152:E152"/>
+    <mergeCell ref="B153:G153"/>
+    <mergeCell ref="B126:E126"/>
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="B110:G110"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B117:E117"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="B125:G125"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="B102:G102"/>
+    <mergeCell ref="B108:G108"/>
+    <mergeCell ref="B109:E109"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B133:G133"/>
     <mergeCell ref="B134:E134"/>
     <mergeCell ref="B135:G135"/>
@@ -15962,51 +16063,9 @@
     <mergeCell ref="B71:G71"/>
     <mergeCell ref="B78:E78"/>
     <mergeCell ref="B79:G79"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="B102:G102"/>
-    <mergeCell ref="B108:G108"/>
-    <mergeCell ref="B109:E109"/>
-    <mergeCell ref="B126:E126"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="B117:E117"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="B125:G125"/>
-    <mergeCell ref="B158:G158"/>
-    <mergeCell ref="B144:E144"/>
-    <mergeCell ref="B145:G145"/>
-    <mergeCell ref="B151:G151"/>
-    <mergeCell ref="B152:E152"/>
-    <mergeCell ref="B153:G153"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F452:F454 F459:F465 F678:F680 F668:F673 F470:F479 F484:F487 F492:F497 F502:F510 F515:F524 F529:F539 F544:F554 F570:F576 F598:F600 F559:F565 F581:F587 F592:F593 F605:F611 F616:F622 F638:F640 F627:F633 F645:F648 F653:F655 F660:F663 F21:F24 F29:F32 F37:F40 F45:F47 F52:F53 F58:F60 F65:F68 F73:F76 F81:F84 F89:F92 F97:F99 F104:F107 F112:F115 F120:F124 F129:F132 F137:F142 F147:F150 F155:F157" xr:uid="{59CD337E-F2A3-4555-8531-BBD5B92517F1}">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F452:F454 F459:F465 F678:F680 F668:F673 F470:F479 F484:F487 F492:F497 F502:F510 F515:F524 F529:F539 F544:F554 F570:F576 F598:F600 F559:F565 F581:F587 F592:F593 F605:F611 F616:F622 F638:F640 F627:F633 F645:F648 F653:F655 F660:F663 F21:F24 F29:F32 F37:F40 F45:F47 F52:F53 F58:F60 F65:F68 F73:F76 F81:F84 F89:F92 F97:F99 F104:F107 F112:F115 F120:F124 F129:F132 F137:F142 F147:F150 F155:F157 F162:F164 F169:F171">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>